<commit_message>
remove database access for test scripts since dev environment will not have db access
refactor tests to work with new processing groups

# Conflicts:
#	apps/forms-flow-ai/forms-flow-web/src/components/FOI/Dashboard/MinistryDashboard.js
</commit_message>
<xml_diff>
--- a/testing/foi-qa-automation/Data Files/Test Data.xlsx
+++ b/testing/foi-qa-automation/Data Files/Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Kan\Katalon Studio\foi-qa-automation\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\foi-flow\testing\foi-qa-automation\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87F41F6-92FF-491C-9BF4-A4902887BCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2F6B26-6C8F-4BBB-A2B4-1AC00DEDADCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="84">
   <si>
     <t>First Name</t>
   </si>
@@ -233,9 +233,6 @@
     <t>foiedu2</t>
   </si>
   <si>
-    <t>personal</t>
-  </si>
-  <si>
     <t>foitac@idir</t>
   </si>
   <si>
@@ -288,6 +285,24 @@
   </si>
   <si>
     <t>Intake - Signed Consent.docx</t>
+  </si>
+  <si>
+    <t>foisocialtech1@idir</t>
+  </si>
+  <si>
+    <t>Social Tech</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>foiflex</t>
+  </si>
+  <si>
+    <t>proxy</t>
   </si>
 </sst>
 </file>
@@ -583,10 +598,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -718,10 +733,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>5</v>
@@ -763,70 +778,87 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>72</v>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -839,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38E4587-88E9-44DF-B2E1-2BCDEAD8E1A1}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -882,7 +914,7 @@
         <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s">
         <v>23</v>
@@ -930,10 +962,10 @@
         <v>34</v>
       </c>
       <c r="U1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -950,7 +982,7 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -989,7 +1021,7 @@
         <v>39</v>
       </c>
       <c r="R2" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="S2" t="s">
         <v>8</v>
@@ -998,10 +1030,10 @@
         <v>19</v>
       </c>
       <c r="U2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="V2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix failing test due axis sync change part 1
</commit_message>
<xml_diff>
--- a/testing/foi-qa-automation/Data Files/Test Data.xlsx
+++ b/testing/foi-qa-automation/Data Files/Test Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\foi-flow\testing\foi-qa-automation\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2F6B26-6C8F-4BBB-A2B4-1AC00DEDADCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D38550B-D6EC-4797-9901-CAE9201533A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>Lastname</t>
   </si>
   <si>
-    <t>a@b.c</t>
-  </si>
-  <si>
     <t>2210 Sooke Rd</t>
   </si>
   <si>
@@ -303,6 +300,9 @@
   </si>
   <si>
     <t>proxy</t>
+  </si>
+  <si>
+    <t>a@b.ca</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -640,12 +640,12 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>7</v>
@@ -654,46 +654,46 @@
         <v>4</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
         <v>40</v>
       </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>7</v>
@@ -702,21 +702,21 @@
         <v>5</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>4</v>
@@ -727,16 +727,16 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>5</v>
@@ -744,121 +744,121 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>52</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>80</v>
-      </c>
       <c r="E15" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38E4587-88E9-44DF-B2E1-2BCDEAD8E1A1}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -902,70 +902,70 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
-        <v>34</v>
-      </c>
       <c r="U1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -976,64 +976,64 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
       </c>
       <c r="L2">
         <v>6041234567</v>
       </c>
       <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
         <v>17</v>
       </c>
-      <c r="N2" t="s">
-        <v>18</v>
-      </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S2" t="s">
         <v>8</v>
       </c>
       <c r="T2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#3391 Organized the folders with respect to review
</commit_message>
<xml_diff>
--- a/testing/foi-qa-automation/Data Files/Test Data.xlsx
+++ b/testing/foi-qa-automation/Data Files/Test Data.xlsx
@@ -10,7 +10,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7miX5KLgZQYx3jc8KpryXV/3NcAvkg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjvWlYXHII17y0QC1CH7z7Ds6UbTg=="/>
     </ext>
   </extLst>
 </workbook>
@@ -37,14 +37,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7misIFgub8kpdu8t5b6TEmvA0N/2tA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mh9UXPVkNTGAeQzAd96ACFS5rQZjA=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="84">
   <si>
     <t>Username</t>
   </si>
@@ -67,7 +67,7 @@
     <t>Foi!123</t>
   </si>
   <si>
-    <t>foiIntake</t>
+    <t>Intake</t>
   </si>
   <si>
     <t>Flex</t>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>foiintakeprocessing@idir</t>
-  </si>
-  <si>
-    <t>Intake</t>
   </si>
   <si>
     <t>Processing</t>
@@ -325,7 +322,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -627,49 +623,49 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
@@ -678,41 +674,41 @@
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>8</v>
@@ -720,121 +716,121 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="E15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1"/>
@@ -1866,138 +1862,138 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="G2" s="4">
         <v>1.0</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="L2" s="4">
         <v>6.041234567E9</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="Q2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="Q2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">

</xml_diff>